<commit_message>
data and return updates
</commit_message>
<xml_diff>
--- a/dataField/dataStorage/my_raw_data.xlsx
+++ b/dataField/dataStorage/my_raw_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunseokjeon/git/yield_calculator/dataField/dataStorage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00326B03-A0EF-F24D-9F52-E22C98C051C9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D55E9430-43EF-4444-84D3-37450CA7900A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32020" yWindow="3060" windowWidth="28100" windowHeight="17440" xr2:uid="{6551E8ED-38DF-1D41-9757-25B6A91C0AFF}"/>
+    <workbookView xWindow="9440" yWindow="2540" windowWidth="28100" windowHeight="17440" xr2:uid="{6551E8ED-38DF-1D41-9757-25B6A91C0AFF}"/>
   </bookViews>
   <sheets>
     <sheet name="시트1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="24">
   <si>
     <t>date</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -115,6 +115,10 @@
   </si>
   <si>
     <t>2018-07-23-월</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2018-10-11-목</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -488,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AB57119-047A-2A43-8CA8-77D96A763DB1}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -779,7 +783,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -796,7 +800,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -811,6 +815,46 @@
       </c>
       <c r="E18">
         <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="3">
+        <v>9190</v>
+      </c>
+      <c r="E19">
+        <v>110</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="3">
+        <v>9200</v>
+      </c>
+      <c r="E20">
+        <v>110</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0.03</v>
       </c>
     </row>
   </sheetData>

</xml_diff>